<commit_message>
acta de scrum 3 y modificacion de la pila de actividades
</commit_message>
<xml_diff>
--- a/Sprint1/Pila de sprint.xlsx
+++ b/Sprint1/Pila de sprint.xlsx
@@ -194,9 +194,6 @@
     <t>Desarrollo de plan de pruebas</t>
   </si>
   <si>
-    <t>Sebastian Marin</t>
-  </si>
-  <si>
     <t>Requerimientos del software</t>
   </si>
   <si>
@@ -429,6 +426,9 @@
   </si>
   <si>
     <t>Sebastián Sanchez</t>
+  </si>
+  <si>
+    <t>Sebastian sanches</t>
   </si>
 </sst>
 </file>
@@ -975,6 +975,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -983,12 +989,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1374,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1386,10 +1386,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
+      <c r="B1" s="56"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1497,66 +1497,66 @@
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="56" t="s">
+      <c r="D6" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="56" t="s">
+      <c r="E6" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="56" t="s">
+      <c r="F6" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="56" t="s">
+      <c r="G6" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="56" t="s">
+      <c r="H6" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="56" t="s">
+      <c r="I6" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="56" t="s">
+      <c r="J6" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="56" t="s">
+      <c r="K6" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="56" t="s">
+      <c r="L6" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="57" t="s">
+      <c r="M6" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="58" t="s">
+      <c r="N6" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="58"/>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="58"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="60"/>
+      <c r="Q6" s="60"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="60"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="56"/>
-      <c r="M7" s="57"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="59"/>
       <c r="N7" s="8" t="s">
         <v>20</v>
       </c>
@@ -1959,13 +1959,13 @@
         <v>33</v>
       </c>
       <c r="F16" s="39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G16" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="39" t="s">
         <v>55</v>
-      </c>
-      <c r="H16" s="39" t="s">
-        <v>56</v>
       </c>
       <c r="I16" s="40">
         <v>43602</v>
@@ -1974,7 +1974,7 @@
         <v>43602</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L16" s="39">
         <v>3</v>
@@ -2037,10 +2037,10 @@
         <v>11</v>
       </c>
       <c r="B18" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="42" t="s">
         <v>57</v>
-      </c>
-      <c r="C18" s="42" t="s">
-        <v>58</v>
       </c>
       <c r="D18" s="32">
         <v>8</v>
@@ -2053,7 +2053,7 @@
       </c>
       <c r="G18" s="32"/>
       <c r="H18" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I18" s="37">
         <v>43606</v>
@@ -2062,16 +2062,18 @@
         <v>43607</v>
       </c>
       <c r="K18" s="33" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="L18" s="25">
         <v>5</v>
       </c>
       <c r="M18" s="18">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="N18" s="34"/>
+        <v>2</v>
+      </c>
+      <c r="N18" s="34">
+        <v>3</v>
+      </c>
       <c r="O18" s="25"/>
       <c r="P18" s="25"/>
       <c r="Q18" s="26"/>
@@ -2081,10 +2083,10 @@
         <v>12</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19" s="32">
         <v>11</v>
@@ -2097,7 +2099,7 @@
       </c>
       <c r="G19" s="32"/>
       <c r="H19" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I19" s="37">
         <v>43607</v>
@@ -2106,16 +2108,18 @@
         <v>43608</v>
       </c>
       <c r="K19" s="33" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="L19" s="25">
         <v>5</v>
       </c>
       <c r="M19" s="18">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="N19" s="34"/>
+        <v>3</v>
+      </c>
+      <c r="N19" s="34">
+        <v>2</v>
+      </c>
       <c r="O19" s="25"/>
       <c r="P19" s="25"/>
       <c r="Q19" s="26"/>
@@ -2125,10 +2129,10 @@
         <v>13</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D20" s="32">
         <v>12</v>
@@ -2141,7 +2145,7 @@
       </c>
       <c r="G20" s="32"/>
       <c r="H20" s="33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I20" s="37">
         <v>43608</v>
@@ -2150,16 +2154,18 @@
         <v>43609</v>
       </c>
       <c r="K20" s="33" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="L20" s="25">
         <v>5</v>
       </c>
       <c r="M20" s="18">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="N20" s="34"/>
+        <v>3</v>
+      </c>
+      <c r="N20" s="34">
+        <v>2</v>
+      </c>
       <c r="O20" s="25"/>
       <c r="P20" s="25"/>
       <c r="Q20" s="26"/>
@@ -2169,10 +2175,10 @@
         <v>14</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D21" s="32">
         <v>13</v>
@@ -2185,7 +2191,7 @@
       </c>
       <c r="G21" s="32"/>
       <c r="H21" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I21" s="37">
         <v>43609</v>
@@ -2194,16 +2200,18 @@
         <v>43610</v>
       </c>
       <c r="K21" s="33" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="L21" s="25">
         <v>3</v>
       </c>
       <c r="M21" s="18">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="N21" s="34"/>
+        <v>2</v>
+      </c>
+      <c r="N21" s="34">
+        <v>1</v>
+      </c>
       <c r="O21" s="25"/>
       <c r="P21" s="25"/>
       <c r="Q21" s="26"/>
@@ -2213,21 +2221,21 @@
         <v>15</v>
       </c>
       <c r="B22" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="39" t="s">
         <v>66</v>
-      </c>
-      <c r="C22" s="39" t="s">
-        <v>67</v>
       </c>
       <c r="D22" s="32"/>
       <c r="E22" s="32">
         <v>5</v>
       </c>
       <c r="F22" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G22" s="32"/>
       <c r="H22" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I22" s="37">
         <v>43612</v>
@@ -2236,7 +2244,7 @@
         <v>43613</v>
       </c>
       <c r="K22" s="33" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="L22" s="25">
         <v>10</v>
@@ -2253,23 +2261,23 @@
     <row r="23" spans="1:17" ht="57" x14ac:dyDescent="0.2">
       <c r="A23" s="43"/>
       <c r="B23" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" s="32"/>
       <c r="E23" s="32">
         <v>5</v>
       </c>
       <c r="F23" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="G23" s="32" t="s">
+      <c r="H23" s="33" t="s">
         <v>72</v>
-      </c>
-      <c r="H23" s="33" t="s">
-        <v>73</v>
       </c>
       <c r="I23" s="36">
         <v>43613</v>
@@ -2278,7 +2286,7 @@
         <v>43614</v>
       </c>
       <c r="K23" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L23" s="25">
         <v>5</v>
@@ -2295,21 +2303,21 @@
     <row r="24" spans="1:17" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A24" s="43"/>
       <c r="B24" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="32" t="s">
         <v>75</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>76</v>
       </c>
       <c r="D24" s="32"/>
       <c r="E24" s="32">
         <v>5</v>
       </c>
       <c r="F24" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G24" s="32"/>
       <c r="H24" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I24" s="37">
         <v>43613</v>
@@ -2318,7 +2326,7 @@
         <v>43615</v>
       </c>
       <c r="K24" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L24" s="25">
         <v>15</v>
@@ -2329,26 +2337,26 @@
       <c r="P24" s="25"/>
       <c r="Q24" s="26"/>
     </row>
-    <row r="25" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="57" x14ac:dyDescent="0.2">
       <c r="A25" s="43"/>
       <c r="B25" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D25" s="32"/>
       <c r="E25" s="32">
         <v>5</v>
       </c>
       <c r="F25" s="32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G25" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" s="33" t="s">
         <v>79</v>
-      </c>
-      <c r="H25" s="33" t="s">
-        <v>80</v>
       </c>
       <c r="I25" s="37">
         <v>43613</v>
@@ -2357,7 +2365,7 @@
         <v>43613</v>
       </c>
       <c r="K25" s="33" t="s">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="L25" s="25">
         <v>2</v>
@@ -2374,23 +2382,23 @@
     <row r="26" spans="1:17" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A26" s="43"/>
       <c r="B26" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D26" s="32"/>
       <c r="E26" s="32">
         <v>5</v>
       </c>
       <c r="F26" s="32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G26" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="H26" s="33" t="s">
         <v>82</v>
-      </c>
-      <c r="H26" s="33" t="s">
-        <v>83</v>
       </c>
       <c r="I26" s="37">
         <v>43614</v>
@@ -2399,7 +2407,7 @@
         <v>43614</v>
       </c>
       <c r="K26" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L26" s="25">
         <v>5</v>
@@ -2416,23 +2424,23 @@
     <row r="27" spans="1:17" ht="57" x14ac:dyDescent="0.2">
       <c r="A27" s="43"/>
       <c r="B27" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D27" s="32"/>
       <c r="E27" s="32">
         <v>4</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G27" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" s="33" t="s">
         <v>85</v>
-      </c>
-      <c r="H27" s="33" t="s">
-        <v>86</v>
       </c>
       <c r="I27" s="37">
         <v>43614</v>
@@ -2441,7 +2449,7 @@
         <v>43615</v>
       </c>
       <c r="K27" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L27" s="25">
         <v>2</v>
@@ -2458,23 +2466,23 @@
     <row r="28" spans="1:17" ht="57" x14ac:dyDescent="0.2">
       <c r="A28" s="44"/>
       <c r="B28" s="45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28" s="45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="45">
         <v>5</v>
       </c>
       <c r="F28" s="45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G28" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="H28" s="46" t="s">
         <v>88</v>
-      </c>
-      <c r="H28" s="46" t="s">
-        <v>89</v>
       </c>
       <c r="I28" s="37">
         <v>43615</v>
@@ -2483,7 +2491,7 @@
         <v>43615</v>
       </c>
       <c r="K28" s="46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L28" s="20">
         <v>2</v>
@@ -2500,23 +2508,23 @@
     <row r="29" spans="1:17" ht="57" x14ac:dyDescent="0.2">
       <c r="A29" s="39"/>
       <c r="B29" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D29" s="32"/>
       <c r="E29" s="32">
         <v>4</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G29" s="32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H29" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I29" s="49">
         <v>43616</v>
@@ -2525,7 +2533,7 @@
         <v>43616</v>
       </c>
       <c r="K29" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L29" s="25">
         <v>3</v>
@@ -2539,23 +2547,23 @@
     <row r="30" spans="1:17" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A30" s="39"/>
       <c r="B30" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" s="32"/>
       <c r="E30" s="32">
         <v>5</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G30" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="H30" s="32" t="s">
         <v>93</v>
-      </c>
-      <c r="H30" s="32" t="s">
-        <v>94</v>
       </c>
       <c r="I30" s="49">
         <v>43616</v>
@@ -2564,7 +2572,7 @@
         <v>43616</v>
       </c>
       <c r="K30" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L30" s="25">
         <v>5</v>
@@ -2578,23 +2586,23 @@
     <row r="31" spans="1:17" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A31" s="39"/>
       <c r="B31" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D31" s="32"/>
       <c r="E31" s="32">
         <v>5</v>
       </c>
       <c r="F31" s="32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G31" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="H31" s="32" t="s">
         <v>96</v>
-      </c>
-      <c r="H31" s="32" t="s">
-        <v>97</v>
       </c>
       <c r="I31" s="49">
         <v>43616</v>
@@ -2603,7 +2611,7 @@
         <v>43616</v>
       </c>
       <c r="K31" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L31" s="25">
         <v>2</v>
@@ -2617,23 +2625,23 @@
     <row r="32" spans="1:17" ht="57" x14ac:dyDescent="0.2">
       <c r="A32" s="39"/>
       <c r="B32" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D32" s="32"/>
       <c r="E32" s="32">
         <v>4</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G32" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="H32" s="32" t="s">
         <v>99</v>
-      </c>
-      <c r="H32" s="32" t="s">
-        <v>100</v>
       </c>
       <c r="I32" s="49">
         <v>43617</v>
@@ -2642,7 +2650,7 @@
         <v>43617</v>
       </c>
       <c r="K32" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L32" s="25">
         <v>3</v>
@@ -2656,21 +2664,21 @@
     <row r="33" spans="1:17" ht="57" x14ac:dyDescent="0.2">
       <c r="A33" s="39"/>
       <c r="B33" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="32" t="s">
         <v>101</v>
-      </c>
-      <c r="C33" s="32" t="s">
-        <v>102</v>
       </c>
       <c r="D33" s="32"/>
       <c r="E33" s="32">
         <v>4</v>
       </c>
       <c r="F33" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G33" s="32"/>
       <c r="H33" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I33" s="49">
         <v>43616</v>
@@ -2679,7 +2687,7 @@
         <v>43616</v>
       </c>
       <c r="K33" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L33" s="25">
         <v>3</v>
@@ -2693,23 +2701,23 @@
     <row r="34" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A34" s="39"/>
       <c r="B34" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D34" s="32"/>
       <c r="E34" s="32">
         <v>3</v>
       </c>
       <c r="F34" s="32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G34" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" s="32" t="s">
         <v>106</v>
-      </c>
-      <c r="H34" s="32" t="s">
-        <v>107</v>
       </c>
       <c r="I34" s="49">
         <v>43616</v>
@@ -2718,7 +2726,7 @@
         <v>43616</v>
       </c>
       <c r="K34" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L34" s="25">
         <v>2</v>
@@ -2732,21 +2740,21 @@
     <row r="35" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A35" s="39"/>
       <c r="B35" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D35" s="32"/>
       <c r="E35" s="32">
         <v>3</v>
       </c>
       <c r="F35" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G35" s="32"/>
       <c r="H35" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I35" s="49">
         <v>43617</v>
@@ -2755,7 +2763,7 @@
         <v>43617</v>
       </c>
       <c r="K35" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L35" s="25">
         <v>3</v>
@@ -2769,23 +2777,23 @@
     <row r="36" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A36" s="41"/>
       <c r="B36" s="51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C36" s="51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D36" s="51"/>
       <c r="E36" s="51">
         <v>3</v>
       </c>
       <c r="F36" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G36" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="H36" s="25" t="s">
         <v>111</v>
-      </c>
-      <c r="H36" s="25" t="s">
-        <v>112</v>
       </c>
       <c r="I36" s="49">
         <v>43617</v>
@@ -2794,7 +2802,7 @@
         <v>43617</v>
       </c>
       <c r="K36" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L36" s="25">
         <v>2</v>
@@ -2808,20 +2816,20 @@
     <row r="37" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A37" s="41"/>
       <c r="B37" s="51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37" s="51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D37" s="51"/>
       <c r="E37" s="51">
         <v>3</v>
       </c>
       <c r="F37" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G37" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H37" s="25"/>
       <c r="I37" s="52">
@@ -2831,7 +2839,7 @@
         <v>43619</v>
       </c>
       <c r="K37" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L37" s="25">
         <v>2</v>
@@ -2863,26 +2871,26 @@
     <row r="39" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A39" s="41"/>
       <c r="B39" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="54" t="s">
         <v>114</v>
-      </c>
-      <c r="C39" s="54" t="s">
-        <v>115</v>
       </c>
       <c r="D39" s="51"/>
       <c r="E39" s="51">
         <v>3</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>54</v>
+        <v>132</v>
       </c>
       <c r="G39" s="25"/>
       <c r="H39" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I39" s="52"/>
       <c r="J39" s="51"/>
       <c r="K39" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L39" s="25"/>
       <c r="M39" s="25"/>
@@ -2895,7 +2903,7 @@
       <c r="A40" s="41"/>
       <c r="B40" s="51"/>
       <c r="C40" s="51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D40" s="51"/>
       <c r="E40" s="51"/>
@@ -2916,7 +2924,7 @@
       <c r="A41" s="41"/>
       <c r="B41" s="51"/>
       <c r="C41" s="51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D41" s="51"/>
       <c r="E41" s="51"/>
@@ -2995,7 +3003,7 @@
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="55" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>33</v>
@@ -3005,7 +3013,7 @@
       <c r="H45" s="41"/>
       <c r="I45" s="41"/>
       <c r="J45" s="55" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K45" s="7" t="s">
         <v>42</v>
@@ -3020,10 +3028,10 @@
     <row r="46" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A46" s="41"/>
       <c r="B46" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>121</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>122</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="7" t="s">
@@ -3048,11 +3056,11 @@
       <c r="A47" s="41"/>
       <c r="B47" s="41"/>
       <c r="C47" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F47" s="41"/>
       <c r="G47" s="41"/>
@@ -3073,11 +3081,11 @@
       <c r="A48" s="41"/>
       <c r="B48" s="41"/>
       <c r="C48" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F48" s="41"/>
       <c r="G48" s="41"/>
@@ -3085,7 +3093,7 @@
       <c r="I48" s="41"/>
       <c r="J48" s="41"/>
       <c r="K48" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L48" s="41"/>
       <c r="M48" s="41"/>
@@ -3102,7 +3110,7 @@
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F49" s="41"/>
       <c r="G49" s="41"/>
@@ -3121,7 +3129,7 @@
       <c r="A50" s="41"/>
       <c r="B50" s="41"/>
       <c r="C50" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="41"/>
@@ -3142,7 +3150,7 @@
       <c r="A51" s="41"/>
       <c r="B51" s="41"/>
       <c r="C51" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="41"/>
@@ -3184,7 +3192,7 @@
       <c r="A53" s="41"/>
       <c r="B53" s="41"/>
       <c r="C53" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="41"/>
@@ -3203,21 +3211,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:Q6"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>